<commit_message>
Projectile Data 기반으로 변경 / PTProjectile와 PTPlayerCharacter 의존성 제거
</commit_message>
<xml_diff>
--- a/GameData/GameData.xlsx
+++ b/GameData/GameData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Unreal\MyProject\Project2\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FD9D06-7D16-4E6E-B930-A5AD13D68EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080115AD-3F29-4A3F-8A7E-EB1787A2B87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3170" windowWidth="19200" windowHeight="11170" activeTab="2" xr2:uid="{B82C8279-B566-4ED0-BB93-2003657E0DE1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{B82C8279-B566-4ED0-BB93-2003657E0DE1}"/>
   </bookViews>
   <sheets>
     <sheet name="PTCharacterStatTable" sheetId="1" r:id="rId1"/>
     <sheet name="PTGunTable" sheetId="3" r:id="rId2"/>
-    <sheet name="PTMonsterStatTable" sheetId="2" r:id="rId3"/>
+    <sheet name="PTProjectileTable" sheetId="4" r:id="rId3"/>
+    <sheet name="PTMonsterStatTable" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>MaxHp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -195,6 +196,30 @@
   </si>
   <si>
     <t>AttackCooldown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExplosionRadius</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Radius</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExplosionEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrailEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExplosionSound</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveSpeed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -683,7 +708,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -853,10 +878,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C036FB-5875-4DAE-94F4-EFECD2FB8E56}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.58203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF759602-E8A5-4A3B-9EAD-436E657575D6}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>